<commit_message>
refactor: update oca (#20)
* feat: id4africa demo

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* resolve conflicts

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* fix: merge conflicts

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* refactor: update schema json

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* refactor: update oca

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

---------

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/credebl/mTech_grade_card/mTech.xlsx
+++ b/OCABundles/schema/credebl/mTech_grade_card/mTech.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="LJzZ/m5GEMbXElkE1DQ96BIHz1PpnE2wmss0ANZJqno="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="vBQHhaCc8pWG+1IxBXxbG9/xI1qa+cHRfjKDGsKrUBc="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t>OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -1163,9 +1163,6 @@
   </si>
   <si>
     <t>University Name</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>University Address</t>
@@ -5458,7 +5455,7 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="71" t="str">
-        <f t="shared" ref="A5:A1003" si="1">IF(AND(NOT(ISBLANK(A$4)),NOT($B5="")),A$4,"")</f>
+        <f t="shared" ref="A5:A1002" si="1">IF(AND(NOT(ISBLANK(A$4)),NOT($B5="")),A$4,"")</f>
         <v/>
       </c>
       <c r="B5" s="77" t="s">
@@ -5798,7 +5795,7 @@
       <c r="Z13" s="49"/>
       <c r="AA13" s="49"/>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
+    <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="71" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5836,7 +5833,7 @@
       <c r="Z14" s="49"/>
       <c r="AA14" s="49"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="71" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5993,16 +5990,10 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B19" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="78" t="s">
-        <v>64</v>
-      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="71"/>
-      <c r="E19" s="74" t="s">
-        <v>100</v>
-      </c>
+      <c r="E19" s="82"/>
       <c r="F19" s="71"/>
       <c r="G19" s="71"/>
       <c r="H19" s="71"/>
@@ -6130,7 +6121,7 @@
       <c r="B23" s="49"/>
       <c r="C23" s="78"/>
       <c r="D23" s="71"/>
-      <c r="E23" s="82"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="71"/>
       <c r="G23" s="71"/>
       <c r="H23" s="71"/>
@@ -6671,7 +6662,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B40" s="49"/>
+      <c r="B40" s="83"/>
       <c r="C40" s="78"/>
       <c r="D40" s="71"/>
       <c r="E40" s="71"/>
@@ -37482,52 +37473,20 @@
       <c r="Z1002" s="49"/>
       <c r="AA1002" s="49"/>
     </row>
-    <row r="1003" ht="12.75" customHeight="1">
-      <c r="A1003" s="71" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B1003" s="83"/>
-      <c r="C1003" s="78"/>
-      <c r="D1003" s="71"/>
-      <c r="E1003" s="71"/>
-      <c r="F1003" s="71"/>
-      <c r="G1003" s="71"/>
-      <c r="H1003" s="71"/>
-      <c r="I1003" s="49"/>
-      <c r="J1003" s="71"/>
-      <c r="K1003" s="81"/>
-      <c r="L1003" s="71"/>
-      <c r="M1003" s="71"/>
-      <c r="N1003" s="71"/>
-      <c r="O1003" s="71"/>
-      <c r="P1003" s="49"/>
-      <c r="Q1003" s="49"/>
-      <c r="R1003" s="49"/>
-      <c r="S1003" s="49"/>
-      <c r="T1003" s="49"/>
-      <c r="U1003" s="49"/>
-      <c r="V1003" s="49"/>
-      <c r="W1003" s="49"/>
-      <c r="X1003" s="49"/>
-      <c r="Y1003" s="49"/>
-      <c r="Z1003" s="49"/>
-      <c r="AA1003" s="49"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:C1003">
+  <conditionalFormatting sqref="C4:C1002">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISBLANK(C4),NOT(ISBLANK(B4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B1003">
+  <conditionalFormatting sqref="B5:B1002">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND(ISBLANK(B5),NOT(SUMPRODUCT(C5:AA5&lt;&gt;"")=0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B1003">
+  <conditionalFormatting sqref="B5:B1002">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISBLANK(B5), SUMPRODUCT(MAX((B5:B1004&lt;&gt;"")*ROW(B5:B1004))) &gt; 0)</formula>
+      <formula>AND(ISBLANK(B5), SUMPRODUCT(MAX((B5:B1003&lt;&gt;"")*ROW(B5:B1003))) &gt; 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
@@ -37537,23 +37496,23 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(B4), SUMPRODUCT(MAX((B4:B1003&lt;&gt;"")*ROW(B4:B1003))) &gt; 0)</formula>
+      <formula>AND(ISBLANK(B4), SUMPRODUCT(MAX((B4:B1002&lt;&gt;"")*ROW(B4:B1002))) &gt; 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L5:L1003">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L5:L1002">
       <formula1>"M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E1003">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4:E1002">
       <formula1>"base64,utf-8,iso-8859-1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D1003">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D1002">
       <formula1>"Y"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="K5:K1003">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="K5:K1002">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C4:C1003">
+    <dataValidation type="list" allowBlank="1" sqref="C4:C1002">
       <formula1>"Binary,Boolean,DateTime,Numeric,Reference,Text,Array[Binary],Array[Boolean],Array[DateTime],Array[Numeric],Array[Reference],Array[Text]"</formula1>
     </dataValidation>
   </dataValidations>
@@ -37600,10 +37559,10 @@
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="86" t="s">
         <v>116</v>
-      </c>
-      <c r="B3" s="86" t="s">
-        <v>117</v>
       </c>
       <c r="C3" s="60" t="s">
         <v>19</v>
@@ -37620,10 +37579,10 @@
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="89" t="s">
         <v>118</v>
-      </c>
-      <c r="B4" s="89" t="s">
-        <v>119</v>
       </c>
       <c r="C4" s="90" t="str">
         <f>IF(ISBLANK(Main!$B4),"",Main!$B4)</f>
@@ -37658,10 +37617,10 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="93" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="93" t="s">
-        <v>121</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>IF(ISBLANK(Main!$B5),"",Main!$B5)</f>
@@ -37935,11 +37894,11 @@
       <c r="B13" s="93"/>
       <c r="C13" s="71" t="str">
         <f>IF(ISBLANK(Main!$B13),"",Main!$B13)</f>
-        <v>Type</v>
+        <v>University Address</v>
       </c>
       <c r="D13" s="71" t="str">
         <f>IF(ISBLANK(Main!$B13),"",Main!$B13)</f>
-        <v>Type</v>
+        <v>University Address</v>
       </c>
       <c r="E13" s="94"/>
       <c r="F13" s="94"/>
@@ -37969,11 +37928,11 @@
       <c r="B14" s="93"/>
       <c r="C14" s="71" t="str">
         <f>IF(ISBLANK(Main!$B14),"",Main!$B14)</f>
-        <v>University Address</v>
+        <v>Semester</v>
       </c>
       <c r="D14" s="71" t="str">
         <f>IF(ISBLANK(Main!$B14),"",Main!$B14)</f>
-        <v>University Address</v>
+        <v>Semester</v>
       </c>
       <c r="E14" s="94"/>
       <c r="F14" s="94"/>
@@ -38003,11 +37962,11 @@
       <c r="B15" s="93"/>
       <c r="C15" s="71" t="str">
         <f>IF(ISBLANK(Main!$B15),"",Main!$B15)</f>
-        <v>Semester</v>
+        <v>Academic Year</v>
       </c>
       <c r="D15" s="71" t="str">
         <f>IF(ISBLANK(Main!$B15),"",Main!$B15)</f>
-        <v>Semester</v>
+        <v>Academic Year</v>
       </c>
       <c r="E15" s="94"/>
       <c r="F15" s="94"/>
@@ -38037,11 +37996,11 @@
       <c r="B16" s="93"/>
       <c r="C16" s="71" t="str">
         <f>IF(ISBLANK(Main!$B16),"",Main!$B16)</f>
-        <v>Academic Year</v>
+        <v>Registration No</v>
       </c>
       <c r="D16" s="71" t="str">
         <f>IF(ISBLANK(Main!$B16),"",Main!$B16)</f>
-        <v>Academic Year</v>
+        <v>Registration No</v>
       </c>
       <c r="E16" s="94"/>
       <c r="F16" s="94"/>
@@ -38071,11 +38030,11 @@
       <c r="B17" s="93"/>
       <c r="C17" s="71" t="str">
         <f>IF(ISBLANK(Main!$B17),"",Main!$B17)</f>
-        <v>Registration No</v>
+        <v>Year</v>
       </c>
       <c r="D17" s="71" t="str">
         <f>IF(ISBLANK(Main!$B17),"",Main!$B17)</f>
-        <v>Registration No</v>
+        <v>Year</v>
       </c>
       <c r="E17" s="94"/>
       <c r="F17" s="94"/>
@@ -38105,11 +38064,11 @@
       <c r="B18" s="93"/>
       <c r="C18" s="71" t="str">
         <f>IF(ISBLANK(Main!$B18),"",Main!$B18)</f>
-        <v>Year</v>
+        <v>Course Details</v>
       </c>
       <c r="D18" s="71" t="str">
         <f>IF(ISBLANK(Main!$B18),"",Main!$B18)</f>
-        <v>Year</v>
+        <v>Course Details</v>
       </c>
       <c r="E18" s="94"/>
       <c r="F18" s="94"/>
@@ -38139,12 +38098,9 @@
       <c r="B19" s="93"/>
       <c r="C19" s="71" t="str">
         <f>IF(ISBLANK(Main!$B19),"",Main!$B19)</f>
-        <v>Course Details</v>
-      </c>
-      <c r="D19" s="71" t="str">
-        <f>IF(ISBLANK(Main!$B19),"",Main!$B19)</f>
-        <v>Course Details</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D19" s="94"/>
       <c r="E19" s="94"/>
       <c r="F19" s="94"/>
       <c r="G19" s="49"/>
@@ -38268,9 +38224,9 @@
         <f>IF(ISBLANK(Main!$B23),"",Main!$B23)</f>
         <v/>
       </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
@@ -68641,46 +68597,15 @@
       <c r="Y1002" s="49"/>
       <c r="Z1002" s="49"/>
     </row>
-    <row r="1003" ht="12.75" customHeight="1">
-      <c r="A1003" s="92"/>
-      <c r="B1003" s="93"/>
-      <c r="C1003" s="71" t="str">
-        <f>IF(ISBLANK(Main!$B1003),"",Main!$B1003)</f>
-        <v/>
-      </c>
-      <c r="D1003" s="71"/>
-      <c r="E1003" s="71"/>
-      <c r="F1003" s="71"/>
-      <c r="G1003" s="49"/>
-      <c r="H1003" s="49"/>
-      <c r="I1003" s="49"/>
-      <c r="J1003" s="49"/>
-      <c r="K1003" s="49"/>
-      <c r="L1003" s="49"/>
-      <c r="M1003" s="49"/>
-      <c r="N1003" s="49"/>
-      <c r="O1003" s="49"/>
-      <c r="P1003" s="49"/>
-      <c r="Q1003" s="49"/>
-      <c r="R1003" s="49"/>
-      <c r="S1003" s="49"/>
-      <c r="T1003" s="49"/>
-      <c r="U1003" s="49"/>
-      <c r="V1003" s="49"/>
-      <c r="W1003" s="49"/>
-      <c r="X1003" s="49"/>
-      <c r="Y1003" s="49"/>
-      <c r="Z1003" s="49"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="E4:F1003 D5 D7 D20:D1003">
+  <conditionalFormatting sqref="E4:F1002 D5 D7 D19:D1002">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(NOT(ISBLANK(E4)),$C4="")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D5 D7 D20:D1003">
-      <formula1>$D$4:$D$1003</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="D5 D7 D19:D1002">
+      <formula1>$D$4:$D$1002</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>

</xml_diff>